<commit_message>
add more transformations and elemental data
</commit_message>
<xml_diff>
--- a/data/elemental.xlsx
+++ b/data/elemental.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dskoda/Dropbox (MIT)/classes/3.321/project/ML/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0526248-B074-0341-A463-0E6EBC3B63FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30039993-A411-2046-8FA7-07766379A17A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29540" yWindow="-740" windowWidth="27240" windowHeight="16040" xr2:uid="{1A04290B-A510-CA4F-B760-1369E11AA8D0}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="38400" windowHeight="17540" xr2:uid="{1A04290B-A510-CA4F-B760-1369E11AA8D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Ce</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>element</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Al</t>
+  </si>
+  <si>
+    <t>Cr</t>
   </si>
 </sst>
 </file>
@@ -463,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F83DBB-6BE8-1442-92BD-41F5DBD893F4}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="170" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -943,6 +952,84 @@
         <v>2.06</v>
       </c>
     </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>0.6</v>
+      </c>
+      <c r="F19">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G19">
+        <v>1.8</v>
+      </c>
+      <c r="H19">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>1.61</v>
+      </c>
+      <c r="C20">
+        <v>0.441</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>1.66</v>
+      </c>
+      <c r="F20">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="G20">
+        <v>1.25</v>
+      </c>
+      <c r="H20">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>1.66</v>
+      </c>
+      <c r="C21">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>0.89</v>
+      </c>
+      <c r="F21">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="G21">
+        <v>1.4</v>
+      </c>
+      <c r="H21">
+        <v>1.66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>